<commit_message>
Updated Route for excel sheet upload
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Riddhi</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>riddhigupta@gmail.com</t>
+  </si>
+  <si>
+    <t>daily_challenge</t>
   </si>
 </sst>
 </file>
@@ -403,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -421,8 +424,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -432,8 +438,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -443,16 +452,22 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -463,12 +478,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Added print statements to debug
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Riddhi</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>daily_challenge</t>
+  </si>
+  <si>
+    <t>answer answer</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +467,7 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -477,10 +480,16 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6">
         <v>3</v>

</xml_diff>

<commit_message>
Added marks to excel sheet
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Riddhi</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>answer answer</t>
+  </si>
+  <si>
+    <t>marks</t>
   </si>
 </sst>
 </file>
@@ -409,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -430,8 +433,11 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,10 +448,13 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -456,10 +465,13 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -469,8 +481,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -481,10 +496,10 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -492,10 +507,10 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>